<commit_message>
enhanced social icons + added notebooks
</commit_message>
<xml_diff>
--- a/ai_plan_klc25.xlsx
+++ b/ai_plan_klc25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haya/Desktop/Desktop - Haya’s MacBook Pro/ai club/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haya/Desktop/Desktop - Haya’s MacBook Pro/ai club/klc-fcitr-planner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8F3F5A6-7A2F-2F48-A85A-5C910DE7D948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C97901F-89F7-5A4F-B36A-9E1A8467F184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="920" windowWidth="27040" windowHeight="15140" xr2:uid="{81604630-A14A-BC4A-B5CA-7D081E8700B9}"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="27040" windowHeight="15140" xr2:uid="{81604630-A14A-BC4A-B5CA-7D081E8700B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="90">
   <si>
     <t>Sun</t>
   </si>
@@ -287,16 +287,25 @@
     <t>colab_link</t>
   </si>
   <si>
-    <t>https://colab.research.google.com/drive/1S69x7V3yykxjTYfK64VlqAuFeeykptii?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://colab.research.google.com/drive/1hyGyrBUaOhoY-dXtqSk6jQRjbAPIYg7T?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://colab.research.google.com/drive/1VL8uZ1NlHvRiILoQ6oj4OEKLz3880DHX?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://colab.research.google.com/drive/1pitU7_EfGQDEvtPnA8k93McVUNdrtY4i?usp=sharing</t>
+    <t>https://colab.research.google.com/drive/1pY5I1gX0frCy5178bvgAOv27vClxF5b8?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://colab.research.google.com/drive/1PpCGfVsALwfuq3YuBXFG9zU6KSHuNVUM?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://colab.research.google.com/drive/1qqzPxSsejvMxF_CcxyvaNYDV3kNAAM6_?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://colab.research.google.com/drive/13-BIk3bh8Py3Asd0o9T1TrbL0QxezU6P?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://colab.research.google.com/drive/1aR7xBhCyoLMo_sfkQeRjwyz7FO6e09CK?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://colab.research.google.com/drive/1Nu7S8G80OL9gpSeOvowtKZjSQ87XbG9V?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://colab.research.google.com/drive/1mai31zBKjwTT7VLbxvil28x_p9kbQGIN?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -839,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DBC7A6-B363-284E-907A-4D4D24EC4F9A}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="92" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1017,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1034,8 +1043,11 @@
         <v>15</v>
       </c>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="J6" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1061,8 +1073,11 @@
         <v>18</v>
       </c>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="J7" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1088,6 +1103,9 @@
         <v>21</v>
       </c>
       <c r="I8" s="5"/>
+      <c r="J8" s="20" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1851,6 +1869,9 @@
     <hyperlink ref="J3" r:id="rId2" xr:uid="{71ADFCDB-132D-BA45-A4A9-56C38613756C}"/>
     <hyperlink ref="J4" r:id="rId3" xr:uid="{C2B74EE6-48F2-E947-B19A-E2168BC0C5C0}"/>
     <hyperlink ref="J5" r:id="rId4" xr:uid="{EDD3AC5A-158C-1D43-87C2-3C718CE4D59B}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{8F736A2F-5A11-D347-B0EB-E06BB577D409}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{5D9E1A43-D7D9-C049-88F4-8A60EA6AB7BC}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{8B0418ED-65CC-4049-AFF8-A902787A31D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>